<commit_message>
Revert "Scrum En Weaponrack"
This reverts commit 2d42a4a0c3f8a54f222cab118d523040dc5b2d97.
</commit_message>
<xml_diff>
--- a/Algemeen/Scrumlog/Invulblad.xlsx
+++ b/Algemeen/Scrumlog/Invulblad.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Week #</t>
   </si>
@@ -77,46 +77,55 @@
     <t>Wat kan er beter</t>
   </si>
   <si>
-    <t>Michiel Sam</t>
-  </si>
-  <si>
-    <t>Carlo Zine Marc Robin Rief</t>
-  </si>
-  <si>
-    <t>Package Fixen &amp; Ak</t>
-  </si>
-  <si>
-    <t>Enemy AI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tafel </t>
-  </si>
-  <si>
-    <t>Inspecting</t>
-  </si>
-  <si>
-    <t>Kalashikov , Calender</t>
-  </si>
-  <si>
-    <t>Enemy Ai Afmaken</t>
-  </si>
-  <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>Butcher Knife , Tafel fix</t>
-  </si>
-  <si>
-    <t>Inspecting , Levelbouw</t>
-  </si>
-  <si>
-    <t>Afwezigheid</t>
-  </si>
-  <si>
-    <t>De collegiale Comunicatie in het fasinerende project.</t>
-  </si>
-  <si>
-    <t>Concerstratie Scrum</t>
+    <t>Carlo Zine Marc Sam</t>
+  </si>
+  <si>
+    <t>Rief , Michiel , Robin</t>
+  </si>
+  <si>
+    <t>Shotgun</t>
+  </si>
+  <si>
+    <t>Gunscript</t>
+  </si>
+  <si>
+    <t>Player Controller</t>
+  </si>
+  <si>
+    <t>unwrap pistol</t>
+  </si>
+  <si>
+    <t>main menu</t>
+  </si>
+  <si>
+    <t>Main Character</t>
+  </si>
+  <si>
+    <t>Muren en Textures</t>
+  </si>
+  <si>
+    <t>Shotgun texture</t>
+  </si>
+  <si>
+    <t>Planning volgen</t>
+  </si>
+  <si>
+    <t>Planning Maken</t>
+  </si>
+  <si>
+    <t>Texture en Animatie</t>
+  </si>
+  <si>
+    <t>Main Character]</t>
+  </si>
+  <si>
+    <t>Waarom zo boos?(-zine)</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
+    <t>Team Spirit</t>
   </si>
 </sst>
 </file>
@@ -601,7 +610,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -629,7 +638,7 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -643,7 +652,7 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -696,7 +705,9 @@
         <v>6</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -709,7 +720,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -723,7 +734,7 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -736,7 +747,9 @@
         <v>9</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -748,7 +761,9 @@
         <v>10</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -773,7 +788,7 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -787,7 +802,7 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -801,7 +816,7 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -815,7 +830,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -829,7 +844,7 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -842,7 +857,9 @@
         <v>9</v>
       </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="9"/>
+      <c r="C19" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -854,7 +871,9 @@
         <v>10</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -878,9 +897,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -892,7 +909,9 @@
         <v>5</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -904,7 +923,9 @@
         <v>6</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -965,7 +986,7 @@
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -988,9 +1009,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="5"/>
-      <c r="C31" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>

</xml_diff>